<commit_message>
10/15/24 932PM from laptop
</commit_message>
<xml_diff>
--- a/2024/Fall 2024/Senior Design 1/Trainer Platform Budget.xlsx
+++ b/2024/Fall 2024/Senior Design 1/Trainer Platform Budget.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brand\Documents\SchoolFiles\2024\Fall 2024\Senior Design 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyl\OneDrive\Documents\SchoolFiles\2024\Fall 2024\Senior Design 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BA8E59-BF3D-454A-8753-564AD6980D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D8DD35-4C1A-409E-A396-FF7F2C6CED74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9C107049-ECFA-4CD5-80D5-387CCB8B6F3A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9C107049-ECFA-4CD5-80D5-387CCB8B6F3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -830,6 +830,39 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
@@ -845,12 +878,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="8" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -860,9 +887,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -872,31 +896,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1236,26 +1236,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C960F79-6C37-4E0C-99B9-6F0772994666}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:H26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1263,21 +1263,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-    </row>
-    <row r="3" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+    </row>
+    <row r="3" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1292,7 +1292,7 @@
       <c r="F3" s="58"/>
       <c r="G3" s="58"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>45571</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1308,150 +1308,150 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+    <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-    </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="49" t="s">
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="38" t="s">
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="40"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="51"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>15</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>20</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>88.16</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>20</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>35.799999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>20</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>63.52</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>23</v>
       </c>
@@ -1585,35 +1585,35 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="41" t="s">
+    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="43">
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="52">
         <f>SUM(H28:H31)</f>
         <v>230.48</v>
       </c>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="45"/>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="46" t="s">
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="54"/>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="48"/>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="55"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="56"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
         <v>15</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
         <v>36</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>41</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>46</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>50</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>53</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>56</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>60</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>62</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>65</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>68</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>72</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="28" t="s">
         <v>85</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="28" t="s">
         <v>83</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>94.5</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="28" t="s">
         <v>77</v>
       </c>
@@ -2017,35 +2017,35 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="41" t="s">
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="42"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="52">
+      <c r="B50" s="39"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="41">
         <f xml:space="preserve"> SUM(H36:H49)</f>
         <v>2154</v>
       </c>
-      <c r="E50" s="53"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="54"/>
-    </row>
-    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="46" t="s">
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="43"/>
+    </row>
+    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B52" s="55"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="55"/>
-      <c r="H52" s="56"/>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="45"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="46"/>
+    </row>
+    <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="18" t="s">
         <v>15</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="22" t="s">
         <v>89</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="28" t="s">
         <v>93</v>
       </c>
@@ -2125,25 +2125,29 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="41" t="s">
+    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="B56" s="42"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="52">
+      <c r="B56" s="39"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="41">
         <f xml:space="preserve"> SUM(H54:H55)</f>
         <v>33</v>
       </c>
-      <c r="E56" s="53"/>
-      <c r="F56" s="53"/>
-      <c r="G56" s="53"/>
-      <c r="H56" s="54"/>
-    </row>
-    <row r="58" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E56" s="42"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="42"/>
+      <c r="H56" s="43"/>
+    </row>
+    <row r="58" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="D3:G3"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="A9:C12"/>
     <mergeCell ref="A56:C56"/>
@@ -2160,10 +2164,6 @@
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="D32:H32"/>
     <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="D3:G3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E55" r:id="rId1" xr:uid="{C2FAC443-A83A-4E8B-8C24-D32691A600F8}"/>
@@ -2185,8 +2185,9 @@
     <hyperlink ref="E28" r:id="rId17" xr:uid="{1326B7F1-8ECA-436C-9A76-5D4F2F27738A}"/>
     <hyperlink ref="E29" r:id="rId18" xr:uid="{81AD01B5-879E-4810-BAD9-882C22DD6A81}"/>
     <hyperlink ref="E31" r:id="rId19" xr:uid="{9EF19729-1DD8-4877-BFCB-9BE6BD1A0AF9}"/>
+    <hyperlink ref="E48" r:id="rId20" display="https://www.automationdirect.com/adc/shopping/catalog/wiring_solutions/ziplink_pre-wired_connection_cables_-a-_modules/connector_-a-_communications_modules_(complete_list)/zl-rtb20?_gl=1*ck8uhv*_up*MQ..&amp;gclid=Cj0KCQjw6oi4BhD1ARIsAL6pox1asPPnva1b8WEFFdhDwEHlsKTxBfCpjn8lT1bh0qMw16HWsjh9LnIaAkbjEALw_wcB" xr:uid="{50345D3D-FF5B-4A16-A4CE-1D90388DEF09}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="55" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId20"/>
+  <pageSetup scale="55" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>